<commit_message>
Fix metabolite name in bootstrap data
</commit_message>
<xml_diff>
--- a/scripts/bootstrap/measurement_data/ri_bt_bh_in_chemostat_controls.xlsx
+++ b/scripts/bootstrap/measurement_data/ri_bt_bh_in_chemostat_controls.xlsx
@@ -58,7 +58,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Measurement time-points in hours (h).</t>
         </r>
@@ -71,7 +70,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Flow-cytometry values per time-point in Cells/mL, use a period (.) as the decimal separator</t>
         </r>
@@ -118,7 +116,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Measurement time-points in hours (h).</t>
         </r>
@@ -131,7 +128,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Abundances values per time-point for strain Roseburia intestinalis, use a period (.) as the decimal separator.</t>
         </r>
@@ -144,7 +140,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Abundances values per time-point for strain Blautia hydrogenotrophica, use a period (.) as the decimal separator.</t>
         </r>
@@ -157,7 +152,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Abundances values per time-point for strain Bacteroides thetaiotaomicron, use a period (.) as the decimal separator.</t>
         </r>
@@ -170,7 +164,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">FC counts values per time-point for strain Roseburia intestinalis in Cells/mL, use a period (.) as the decimal separator</t>
         </r>
@@ -183,7 +176,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">FC counts values per time-point for strain Blautia hydrogenotrophica in Cells/mL, use a period (.) as the decimal separator</t>
         </r>
@@ -196,7 +188,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">FC counts values per time-point for strain Bacteroides thetaiotaomicron in Cells/mL, use a period (.) as the decimal separator</t>
         </r>
@@ -243,7 +234,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Measurement time-points in hours (h).</t>
         </r>
@@ -256,7 +246,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Concentration values per time-point for metabolite acetic acid in mM, use a period (.) as the decimal separator</t>
         </r>
@@ -269,7 +258,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Concentration values per time-point for metabolite succinic acid in mM, use a period (.) as the decimal separator</t>
         </r>
@@ -282,7 +270,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Concentration values per time-point for metabolite glucose in mM, use a period (.) as the decimal separator</t>
         </r>
@@ -295,7 +282,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Concentration values per time-point for metabolite trehalose in mM, use a period (.) as the decimal separator</t>
         </r>
@@ -308,7 +294,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Concentration values per time-point for metabolite formic acid in mM, use a period (.) as the decimal separator</t>
         </r>
@@ -321,7 +306,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Concentration values per time-point for metabolite butyric acid in mM, use a period (.) as the decimal separator</t>
         </r>
@@ -334,7 +318,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Concentration values per time-point for metabolite pyruvic acid in mM, use a period (.) as the decimal separator</t>
         </r>
@@ -347,7 +330,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Concentration values per time-point for metabolite (s)-lactic acid in mM, use a period (.) as the decimal separator</t>
         </r>
@@ -432,7 +414,7 @@
     <t xml:space="preserve">pyruvic acid</t>
   </si>
   <si>
-    <t xml:space="preserve">(s)-lactic acid</t>
+    <t xml:space="preserve">(S)-lactic acid</t>
   </si>
 </sst>
 </file>
@@ -444,7 +426,7 @@
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,12 +468,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -591,7 +567,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -611,7 +587,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -623,11 +599,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -895,13 +871,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D:K"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.48"/>
   </cols>
@@ -921,10 +897,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="n">
@@ -935,10 +911,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="6" t="n">
@@ -949,10 +925,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="6" t="n">
@@ -963,10 +939,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="6" t="n">
@@ -977,10 +953,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="6" t="n">
@@ -991,10 +967,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="6" t="n">
@@ -1005,10 +981,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="6" t="n">
@@ -1019,10 +995,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6" t="n">
@@ -1047,10 +1023,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="4" t="n">
@@ -1061,10 +1037,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="6" t="n">
@@ -1075,10 +1051,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="6" t="n">
@@ -1089,10 +1065,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="6" t="n">
@@ -1103,10 +1079,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="6" t="n">
@@ -1117,10 +1093,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="6" t="n">
@@ -1131,10 +1107,10 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="6" t="n">
@@ -1145,10 +1121,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="6" t="n">
@@ -1173,10 +1149,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="4" t="n">
@@ -1187,10 +1163,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="6" t="n">
@@ -1201,10 +1177,10 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6" t="n">
@@ -1215,10 +1191,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="6" t="n">
@@ -1229,10 +1205,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="6" t="n">
@@ -1243,10 +1219,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="6" t="n">
@@ -1257,10 +1233,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="6" t="n">
@@ -1271,10 +1247,10 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="6" t="n">
@@ -1299,10 +1275,10 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="4" t="n">
@@ -1313,10 +1289,10 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="6" t="n">
@@ -1327,10 +1303,10 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="6" t="n">
@@ -1341,10 +1317,10 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="6" t="n">
@@ -1355,10 +1331,10 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="6" t="n">
@@ -1369,10 +1345,10 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="6" t="n">
@@ -1383,10 +1359,10 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="6" t="n">
@@ -1397,10 +1373,10 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="6" t="n">
@@ -1425,10 +1401,10 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="4" t="n">
@@ -1439,10 +1415,10 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="6" t="n">
@@ -1453,10 +1429,10 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="6" t="n">
@@ -1467,10 +1443,10 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="6" t="n">
@@ -1481,10 +1457,10 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="6" t="n">
@@ -1495,10 +1471,10 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="6" t="n">
@@ -1509,10 +1485,10 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C44" s="6" t="n">
@@ -1523,10 +1499,10 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C45" s="6" t="n">
@@ -1551,10 +1527,10 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C47" s="4" t="n">
@@ -1565,10 +1541,10 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C48" s="6" t="n">
@@ -1579,10 +1555,10 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="6" t="n">
@@ -1593,10 +1569,10 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="6" t="n">
@@ -1607,10 +1583,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="6" t="n">
@@ -1621,10 +1597,10 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C52" s="6" t="n">
@@ -1635,10 +1611,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="6" t="n">
@@ -1649,10 +1625,10 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C54" s="6" t="n">
@@ -1700,13 +1676,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D:K"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.99"/>
@@ -1746,10 +1722,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="n">
@@ -1775,10 +1751,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="6" t="n">
@@ -1804,10 +1780,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="6" t="n">
@@ -1833,10 +1809,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="6" t="n">
@@ -1850,10 +1826,10 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="6" t="n">
@@ -1879,10 +1855,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="6" t="n">
@@ -1908,10 +1884,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="6" t="n">
@@ -1937,10 +1913,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6" t="n">
@@ -1995,10 +1971,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="4" t="n">
@@ -2024,10 +2000,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="6" t="n">
@@ -2053,10 +2029,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="6" t="n">
@@ -2082,10 +2058,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="6" t="n">
@@ -2099,10 +2075,10 @@
       <c r="I14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="6" t="n">
@@ -2128,10 +2104,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="6" t="n">
@@ -2157,10 +2133,10 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="6" t="n">
@@ -2186,10 +2162,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="6" t="n">
@@ -2244,10 +2220,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="4" t="n">
@@ -2273,10 +2249,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="6" t="n">
@@ -2302,10 +2278,10 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6" t="n">
@@ -2331,10 +2307,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="6" t="n">
@@ -2360,10 +2336,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="6" t="n">
@@ -2389,10 +2365,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="6" t="n">
@@ -2418,10 +2394,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="6" t="n">
@@ -2447,10 +2423,10 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="6" t="n">
@@ -2505,10 +2481,10 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="4" t="n">
@@ -2534,10 +2510,10 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="6" t="n">
@@ -2563,10 +2539,10 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="6" t="n">
@@ -2592,10 +2568,10 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="6" t="n">
@@ -2621,10 +2597,10 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="6" t="n">
@@ -2650,10 +2626,10 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="6" t="n">
@@ -2679,10 +2655,10 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="6" t="n">
@@ -2708,10 +2684,10 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="6" t="n">
@@ -2766,10 +2742,10 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="4" t="n">
@@ -2795,10 +2771,10 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="6" t="n">
@@ -2824,10 +2800,10 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="6" t="n">
@@ -2853,10 +2829,10 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="6" t="n">
@@ -2882,10 +2858,10 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="6" t="n">
@@ -2911,10 +2887,10 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="6" t="n">
@@ -2940,10 +2916,10 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C44" s="6" t="n">
@@ -2969,10 +2945,10 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C45" s="6" t="n">
@@ -3027,10 +3003,10 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C47" s="4" t="n">
@@ -3056,10 +3032,10 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C48" s="6" t="n">
@@ -3085,10 +3061,10 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="6" t="n">
@@ -3114,10 +3090,10 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="6" t="n">
@@ -3143,10 +3119,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="6" t="n">
@@ -3172,10 +3148,10 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C52" s="6" t="n">
@@ -3201,10 +3177,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="6" t="n">
@@ -3230,10 +3206,10 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C54" s="6" t="n">
@@ -3307,17 +3283,17 @@
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D:K"/>
+      <selection pane="bottomRight" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19"/>
@@ -3364,10 +3340,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="n">
@@ -3399,10 +3375,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="6" t="n">
@@ -3434,10 +3410,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="6" t="n">
@@ -3469,10 +3445,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="6" t="n">
@@ -3504,10 +3480,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="6" t="n">
@@ -3539,10 +3515,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="6" t="n">
@@ -3574,10 +3550,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="6" t="n">
@@ -3609,10 +3585,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6" t="n">
@@ -3679,10 +3655,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="4" t="n">
@@ -3698,10 +3674,10 @@
       <c r="K11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="6" t="n">
@@ -3717,10 +3693,10 @@
       <c r="K12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="6" t="n">
@@ -3736,10 +3712,10 @@
       <c r="K13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="6" t="n">
@@ -3755,10 +3731,10 @@
       <c r="K14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="6" t="n">
@@ -3774,10 +3750,10 @@
       <c r="K15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="6" t="n">
@@ -3793,10 +3769,10 @@
       <c r="K16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="6" t="n">
@@ -3812,10 +3788,10 @@
       <c r="K17" s="12"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="6" t="n">
@@ -3850,10 +3826,10 @@
       <c r="K19" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="4" t="n">
@@ -3885,10 +3861,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="6" t="n">
@@ -3920,10 +3896,10 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6" t="n">
@@ -3955,10 +3931,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="6" t="n">
@@ -3990,10 +3966,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="6" t="n">
@@ -4025,10 +4001,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="6" t="n">
@@ -4060,10 +4036,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="6" t="n">
@@ -4095,10 +4071,10 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="6" t="n">
@@ -4165,10 +4141,10 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="4" t="n">
@@ -4184,10 +4160,10 @@
       <c r="K29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="6" t="n">
@@ -4203,10 +4179,10 @@
       <c r="K30" s="12"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="6" t="n">
@@ -4222,10 +4198,10 @@
       <c r="K31" s="12"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="6" t="n">
@@ -4241,10 +4217,10 @@
       <c r="K32" s="12"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="6" t="n">
@@ -4260,10 +4236,10 @@
       <c r="K33" s="12"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="6" t="n">
@@ -4279,10 +4255,10 @@
       <c r="K34" s="12"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="6" t="n">
@@ -4298,10 +4274,10 @@
       <c r="K35" s="12"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="6" t="n">
@@ -4336,10 +4312,10 @@
       <c r="K37" s="12"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="4" t="n">
@@ -4371,10 +4347,10 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="6" t="n">
@@ -4406,10 +4382,10 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="6" t="n">
@@ -4441,10 +4417,10 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="6" t="n">
@@ -4476,10 +4452,10 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="6" t="n">
@@ -4511,10 +4487,10 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="6" t="n">
@@ -4546,10 +4522,10 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C44" s="6" t="n">
@@ -4581,10 +4557,10 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C45" s="6" t="n">
@@ -4651,10 +4627,10 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C47" s="4" t="n">
@@ -4662,10 +4638,10 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C48" s="6" t="n">
@@ -4673,10 +4649,10 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="6" t="n">
@@ -4684,10 +4660,10 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="6" t="n">
@@ -4695,10 +4671,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="6" t="n">
@@ -4706,10 +4682,10 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C52" s="6" t="n">
@@ -4717,10 +4693,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="6" t="n">
@@ -4728,10 +4704,10 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C54" s="6" t="n">

</xml_diff>

<commit_message>
Add pH data to S3
</commit_message>
<xml_diff>
--- a/scripts/bootstrap/measurement_data/ri_bt_bh_in_chemostat_controls.xlsx
+++ b/scripts/bootstrap/measurement_data/ri_bt_bh_in_chemostat_controls.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Growth data per community" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Growth data per strain" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Growth data per metabolite" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Community pH" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -340,7 +341,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="26">
   <si>
     <t xml:space="preserve">Biological Replicate</t>
   </si>
@@ -415,6 +416,9 @@
   </si>
   <si>
     <t xml:space="preserve">(S)-lactic acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Community pH</t>
   </si>
 </sst>
 </file>
@@ -871,7 +875,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="A1:D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1671,12 +1675,12 @@
   </sheetPr>
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G9" activeCellId="1" sqref="A1:D103 G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3287,7 +3291,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="K2" activeCellId="1" sqref="A1:D103 K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4735,4 +4739,1477 @@
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="1" sqref="A1:D103 F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.484375" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.87"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>6.41</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>5.96</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>246</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>5.76</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>5.76</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>342</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>5.76</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>390</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>6.41</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>5.89</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>5.72</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>246</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>342</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>390</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>6.42</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>5.87</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>5.72</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>246</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>5.82</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>5.76</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>342</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>390</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>6.42</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>5.72</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>5.72</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>246</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>5.76</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>342</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>390</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>6.41</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>5.92</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>6.01</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>246</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>5.72</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>5.72</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>342</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>390</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>5.76</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>5.89</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>5.93</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>246</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="D100" s="0" t="n">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>342</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="D102" s="0" t="n">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" s="0" t="n">
+        <v>390</v>
+      </c>
+      <c r="D103" s="0" t="n">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>